<commit_message>
Add test results with more configs
</commit_message>
<xml_diff>
--- a/TestResults_v2_2.xlsx
+++ b/TestResults_v2_2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" activeTab="4"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="1m" sheetId="3" r:id="rId1"/>
@@ -22,13 +22,14 @@
     <sheet name="max 20" sheetId="14" r:id="rId13"/>
     <sheet name="max 25" sheetId="15" r:id="rId14"/>
     <sheet name="max 30" sheetId="16" r:id="rId15"/>
+    <sheet name="All Configs" sheetId="17" r:id="rId16"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="27">
   <si>
     <t>System 1</t>
   </si>
@@ -79,6 +80,36 @@
   </si>
   <si>
     <t>Maximum Debris:</t>
+  </si>
+  <si>
+    <t>System 6</t>
+  </si>
+  <si>
+    <t>System 7</t>
+  </si>
+  <si>
+    <t>System 8</t>
+  </si>
+  <si>
+    <t>System 9</t>
+  </si>
+  <si>
+    <t>System 10</t>
+  </si>
+  <si>
+    <t>System 11</t>
+  </si>
+  <si>
+    <t>System 12</t>
+  </si>
+  <si>
+    <t>System 13</t>
+  </si>
+  <si>
+    <t>System 14</t>
+  </si>
+  <si>
+    <t>System 15</t>
   </si>
 </sst>
 </file>
@@ -4816,6 +4847,3455 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AF57"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="X22" sqref="X22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.85546875" customWidth="1"/>
+    <col min="2" max="2" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:32" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1"/>
+      <c r="B1"/>
+      <c r="C1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4"/>
+      <c r="S1" s="4"/>
+      <c r="T1" s="4"/>
+      <c r="U1" s="4"/>
+      <c r="V1" s="5"/>
+    </row>
+    <row r="2" spans="1:32" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="7">
+        <v>1</v>
+      </c>
+      <c r="D2" s="8">
+        <v>2</v>
+      </c>
+      <c r="E2" s="8">
+        <v>3</v>
+      </c>
+      <c r="F2" s="8">
+        <v>4</v>
+      </c>
+      <c r="G2" s="8">
+        <v>5</v>
+      </c>
+      <c r="H2" s="8">
+        <v>6</v>
+      </c>
+      <c r="I2" s="8">
+        <v>7</v>
+      </c>
+      <c r="J2" s="8">
+        <v>8</v>
+      </c>
+      <c r="K2" s="8">
+        <v>9</v>
+      </c>
+      <c r="L2" s="8">
+        <v>10</v>
+      </c>
+      <c r="M2" s="8">
+        <v>11</v>
+      </c>
+      <c r="N2" s="8">
+        <v>12</v>
+      </c>
+      <c r="O2" s="8">
+        <v>13</v>
+      </c>
+      <c r="P2" s="8">
+        <v>14</v>
+      </c>
+      <c r="Q2" s="8">
+        <v>15</v>
+      </c>
+      <c r="R2" s="8">
+        <v>16</v>
+      </c>
+      <c r="S2" s="8">
+        <v>17</v>
+      </c>
+      <c r="T2" s="8">
+        <v>18</v>
+      </c>
+      <c r="U2" s="8">
+        <v>19</v>
+      </c>
+      <c r="V2" s="9">
+        <v>20</v>
+      </c>
+      <c r="W2" s="12"/>
+      <c r="X2" s="12"/>
+      <c r="Y2" s="12"/>
+      <c r="Z2" s="12"/>
+      <c r="AA2" s="12"/>
+      <c r="AB2" s="12"/>
+      <c r="AC2" s="12"/>
+      <c r="AD2" s="12"/>
+      <c r="AE2" s="12"/>
+      <c r="AF2" s="12"/>
+    </row>
+    <row r="3" spans="1:32" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="6">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3" s="11">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
+      <c r="T3">
+        <v>0</v>
+      </c>
+      <c r="U3">
+        <v>0</v>
+      </c>
+      <c r="V3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:32" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4"/>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4" s="10">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4">
+        <v>0</v>
+      </c>
+      <c r="U4">
+        <v>0</v>
+      </c>
+      <c r="V4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5" s="10">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="T5">
+        <v>0</v>
+      </c>
+      <c r="U5">
+        <v>0</v>
+      </c>
+      <c r="V5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6" s="10">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
+      <c r="R6">
+        <v>0</v>
+      </c>
+      <c r="S6">
+        <v>0</v>
+      </c>
+      <c r="T6">
+        <v>0</v>
+      </c>
+      <c r="U6">
+        <v>0</v>
+      </c>
+      <c r="V6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7" s="10">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+      <c r="R7">
+        <v>0</v>
+      </c>
+      <c r="S7">
+        <v>0</v>
+      </c>
+      <c r="T7">
+        <v>0</v>
+      </c>
+      <c r="U7">
+        <v>0</v>
+      </c>
+      <c r="V7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8" s="10">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+      <c r="Q8">
+        <v>0</v>
+      </c>
+      <c r="R8">
+        <v>0</v>
+      </c>
+      <c r="S8">
+        <v>0</v>
+      </c>
+      <c r="T8">
+        <v>0</v>
+      </c>
+      <c r="U8">
+        <v>0</v>
+      </c>
+      <c r="V8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9" s="10">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="Q9">
+        <v>0</v>
+      </c>
+      <c r="R9">
+        <v>0</v>
+      </c>
+      <c r="S9">
+        <v>0</v>
+      </c>
+      <c r="T9">
+        <v>0</v>
+      </c>
+      <c r="U9">
+        <v>0</v>
+      </c>
+      <c r="V9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10" s="10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+      <c r="Q10">
+        <v>0</v>
+      </c>
+      <c r="R10">
+        <v>0</v>
+      </c>
+      <c r="S10">
+        <v>0</v>
+      </c>
+      <c r="T10">
+        <v>0</v>
+      </c>
+      <c r="U10">
+        <v>0</v>
+      </c>
+      <c r="V10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11" s="10">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+      <c r="Q11">
+        <v>0</v>
+      </c>
+      <c r="R11">
+        <v>0</v>
+      </c>
+      <c r="S11">
+        <v>0</v>
+      </c>
+      <c r="T11">
+        <v>0</v>
+      </c>
+      <c r="U11">
+        <v>0</v>
+      </c>
+      <c r="V11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="2">
+        <v>1.5306120000000001</v>
+      </c>
+      <c r="D12">
+        <v>1.5306120000000001</v>
+      </c>
+      <c r="E12">
+        <v>1.5306120000000001</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12" s="10">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
+      <c r="Q12">
+        <v>0</v>
+      </c>
+      <c r="R12">
+        <v>0</v>
+      </c>
+      <c r="S12">
+        <v>0</v>
+      </c>
+      <c r="T12">
+        <v>0</v>
+      </c>
+      <c r="U12">
+        <v>0</v>
+      </c>
+      <c r="V12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="2">
+        <v>17.99999712</v>
+      </c>
+      <c r="D13">
+        <v>17.99999712</v>
+      </c>
+      <c r="E13">
+        <v>17.99999712</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13" s="10">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <v>0</v>
+      </c>
+      <c r="P13">
+        <v>0</v>
+      </c>
+      <c r="Q13">
+        <v>0</v>
+      </c>
+      <c r="R13">
+        <v>0</v>
+      </c>
+      <c r="S13">
+        <v>0</v>
+      </c>
+      <c r="T13">
+        <v>0</v>
+      </c>
+      <c r="U13">
+        <v>0</v>
+      </c>
+      <c r="V13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="2">
+        <v>17.99999712</v>
+      </c>
+      <c r="D14">
+        <v>35.999994239999999</v>
+      </c>
+      <c r="E14">
+        <v>53.999991360000003</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14" s="10">
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <v>0</v>
+      </c>
+      <c r="P14">
+        <v>0</v>
+      </c>
+      <c r="Q14">
+        <v>0</v>
+      </c>
+      <c r="R14">
+        <v>0</v>
+      </c>
+      <c r="S14">
+        <v>0</v>
+      </c>
+      <c r="T14">
+        <v>0</v>
+      </c>
+      <c r="U14">
+        <v>0</v>
+      </c>
+      <c r="V14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="2">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15" s="10">
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <v>0</v>
+      </c>
+      <c r="P15">
+        <v>0</v>
+      </c>
+      <c r="Q15">
+        <v>0</v>
+      </c>
+      <c r="R15">
+        <v>0</v>
+      </c>
+      <c r="S15">
+        <v>0</v>
+      </c>
+      <c r="T15">
+        <v>0</v>
+      </c>
+      <c r="U15">
+        <v>0</v>
+      </c>
+      <c r="V15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="2">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16" s="10">
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <v>0</v>
+      </c>
+      <c r="P16">
+        <v>0</v>
+      </c>
+      <c r="Q16">
+        <v>0</v>
+      </c>
+      <c r="R16">
+        <v>0</v>
+      </c>
+      <c r="S16">
+        <v>0</v>
+      </c>
+      <c r="T16">
+        <v>0</v>
+      </c>
+      <c r="U16">
+        <v>0</v>
+      </c>
+      <c r="V16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="2">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17" s="10">
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+      <c r="N17">
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <v>0</v>
+      </c>
+      <c r="P17">
+        <v>0</v>
+      </c>
+      <c r="Q17">
+        <v>0</v>
+      </c>
+      <c r="R17">
+        <v>0</v>
+      </c>
+      <c r="S17">
+        <v>0</v>
+      </c>
+      <c r="T17">
+        <v>0</v>
+      </c>
+      <c r="U17">
+        <v>0</v>
+      </c>
+      <c r="V17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="2">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18" s="10">
+        <v>0</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
+      <c r="N18">
+        <v>0</v>
+      </c>
+      <c r="O18">
+        <v>0</v>
+      </c>
+      <c r="P18">
+        <v>0</v>
+      </c>
+      <c r="Q18">
+        <v>0</v>
+      </c>
+      <c r="R18">
+        <v>0</v>
+      </c>
+      <c r="S18">
+        <v>0</v>
+      </c>
+      <c r="T18">
+        <v>0</v>
+      </c>
+      <c r="U18">
+        <v>0</v>
+      </c>
+      <c r="V18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="2">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="L19" s="10">
+        <v>0</v>
+      </c>
+      <c r="M19">
+        <v>0</v>
+      </c>
+      <c r="N19">
+        <v>0</v>
+      </c>
+      <c r="O19">
+        <v>0</v>
+      </c>
+      <c r="P19">
+        <v>0</v>
+      </c>
+      <c r="Q19">
+        <v>0</v>
+      </c>
+      <c r="R19">
+        <v>0</v>
+      </c>
+      <c r="S19">
+        <v>0</v>
+      </c>
+      <c r="T19">
+        <v>0</v>
+      </c>
+      <c r="U19">
+        <v>0</v>
+      </c>
+      <c r="V19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="2">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <v>0</v>
+      </c>
+      <c r="L20" s="10">
+        <v>0</v>
+      </c>
+      <c r="M20">
+        <v>0</v>
+      </c>
+      <c r="N20">
+        <v>0</v>
+      </c>
+      <c r="O20">
+        <v>0</v>
+      </c>
+      <c r="P20">
+        <v>0</v>
+      </c>
+      <c r="Q20">
+        <v>0</v>
+      </c>
+      <c r="R20">
+        <v>0</v>
+      </c>
+      <c r="S20">
+        <v>0</v>
+      </c>
+      <c r="T20">
+        <v>0</v>
+      </c>
+      <c r="U20">
+        <v>0</v>
+      </c>
+      <c r="V20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" s="2">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <v>0</v>
+      </c>
+      <c r="L21" s="10">
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <v>0</v>
+      </c>
+      <c r="N21">
+        <v>0</v>
+      </c>
+      <c r="O21">
+        <v>0</v>
+      </c>
+      <c r="P21">
+        <v>0</v>
+      </c>
+      <c r="Q21">
+        <v>0</v>
+      </c>
+      <c r="R21">
+        <v>0</v>
+      </c>
+      <c r="S21">
+        <v>0</v>
+      </c>
+      <c r="T21">
+        <v>0</v>
+      </c>
+      <c r="U21">
+        <v>0</v>
+      </c>
+      <c r="V21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" s="2">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <v>0</v>
+      </c>
+      <c r="K22">
+        <v>0</v>
+      </c>
+      <c r="L22" s="10">
+        <v>0</v>
+      </c>
+      <c r="M22">
+        <v>0</v>
+      </c>
+      <c r="N22">
+        <v>0</v>
+      </c>
+      <c r="O22">
+        <v>0</v>
+      </c>
+      <c r="P22">
+        <v>0</v>
+      </c>
+      <c r="Q22">
+        <v>0</v>
+      </c>
+      <c r="R22">
+        <v>0</v>
+      </c>
+      <c r="S22">
+        <v>0</v>
+      </c>
+      <c r="T22">
+        <v>0</v>
+      </c>
+      <c r="U22">
+        <v>0</v>
+      </c>
+      <c r="V22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23" s="2">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="K23">
+        <v>0</v>
+      </c>
+      <c r="L23" s="10">
+        <v>0</v>
+      </c>
+      <c r="M23">
+        <v>0</v>
+      </c>
+      <c r="N23">
+        <v>0</v>
+      </c>
+      <c r="O23">
+        <v>0</v>
+      </c>
+      <c r="P23">
+        <v>0</v>
+      </c>
+      <c r="Q23">
+        <v>0</v>
+      </c>
+      <c r="R23">
+        <v>0</v>
+      </c>
+      <c r="S23">
+        <v>0</v>
+      </c>
+      <c r="T23">
+        <v>0</v>
+      </c>
+      <c r="U23">
+        <v>0</v>
+      </c>
+      <c r="V23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>19</v>
+      </c>
+      <c r="B24" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" s="2">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <v>0</v>
+      </c>
+      <c r="K24">
+        <v>0</v>
+      </c>
+      <c r="L24" s="10">
+        <v>0</v>
+      </c>
+      <c r="M24">
+        <v>0</v>
+      </c>
+      <c r="N24">
+        <v>0</v>
+      </c>
+      <c r="O24">
+        <v>0</v>
+      </c>
+      <c r="P24">
+        <v>0</v>
+      </c>
+      <c r="Q24">
+        <v>0</v>
+      </c>
+      <c r="R24">
+        <v>0</v>
+      </c>
+      <c r="S24">
+        <v>0</v>
+      </c>
+      <c r="T24">
+        <v>0</v>
+      </c>
+      <c r="U24">
+        <v>0</v>
+      </c>
+      <c r="V24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" s="2">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <v>0</v>
+      </c>
+      <c r="K25">
+        <v>0</v>
+      </c>
+      <c r="L25" s="10">
+        <v>0</v>
+      </c>
+      <c r="M25">
+        <v>0</v>
+      </c>
+      <c r="N25">
+        <v>0</v>
+      </c>
+      <c r="O25">
+        <v>0</v>
+      </c>
+      <c r="P25">
+        <v>0</v>
+      </c>
+      <c r="Q25">
+        <v>0</v>
+      </c>
+      <c r="R25">
+        <v>0</v>
+      </c>
+      <c r="S25">
+        <v>0</v>
+      </c>
+      <c r="T25">
+        <v>0</v>
+      </c>
+      <c r="U25">
+        <v>0</v>
+      </c>
+      <c r="V25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>7</v>
+      </c>
+      <c r="C26" s="2">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <v>0</v>
+      </c>
+      <c r="J26">
+        <v>0</v>
+      </c>
+      <c r="K26">
+        <v>0</v>
+      </c>
+      <c r="L26" s="10">
+        <v>0</v>
+      </c>
+      <c r="M26">
+        <v>0</v>
+      </c>
+      <c r="N26">
+        <v>0</v>
+      </c>
+      <c r="O26">
+        <v>0</v>
+      </c>
+      <c r="P26">
+        <v>0</v>
+      </c>
+      <c r="Q26">
+        <v>0</v>
+      </c>
+      <c r="R26">
+        <v>0</v>
+      </c>
+      <c r="S26">
+        <v>0</v>
+      </c>
+      <c r="T26">
+        <v>0</v>
+      </c>
+      <c r="U26">
+        <v>0</v>
+      </c>
+      <c r="V26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>20</v>
+      </c>
+      <c r="B27" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27" s="2">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <v>1.5306120000000001</v>
+      </c>
+      <c r="G27">
+        <v>1.5306120000000001</v>
+      </c>
+      <c r="H27">
+        <v>1.5306120000000001</v>
+      </c>
+      <c r="I27">
+        <v>1.5306120000000001</v>
+      </c>
+      <c r="J27">
+        <v>1.5306120000000001</v>
+      </c>
+      <c r="K27">
+        <v>1.5306120000000001</v>
+      </c>
+      <c r="L27" s="10">
+        <v>1.5306120000000001</v>
+      </c>
+      <c r="M27">
+        <v>1.5306120000000001</v>
+      </c>
+      <c r="N27">
+        <v>1.5306120000000001</v>
+      </c>
+      <c r="O27">
+        <v>1.5306120000000001</v>
+      </c>
+      <c r="P27">
+        <v>1.5306120000000001</v>
+      </c>
+      <c r="Q27">
+        <v>1.5306120000000001</v>
+      </c>
+      <c r="R27">
+        <v>1.5306120000000001</v>
+      </c>
+      <c r="S27">
+        <v>1.5306120000000001</v>
+      </c>
+      <c r="T27">
+        <v>1.5306120000000001</v>
+      </c>
+      <c r="U27">
+        <v>1.5306120000000001</v>
+      </c>
+      <c r="V27">
+        <v>1.5306120000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" s="2">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <v>17.99999712</v>
+      </c>
+      <c r="G28">
+        <v>17.99999712</v>
+      </c>
+      <c r="H28">
+        <v>17.99999712</v>
+      </c>
+      <c r="I28">
+        <v>17.99999712</v>
+      </c>
+      <c r="J28">
+        <v>17.99999712</v>
+      </c>
+      <c r="K28">
+        <v>17.99999712</v>
+      </c>
+      <c r="L28" s="10">
+        <v>17.99999712</v>
+      </c>
+      <c r="M28">
+        <v>17.99999712</v>
+      </c>
+      <c r="N28">
+        <v>17.99999712</v>
+      </c>
+      <c r="O28">
+        <v>17.99999712</v>
+      </c>
+      <c r="P28">
+        <v>17.99999712</v>
+      </c>
+      <c r="Q28">
+        <v>17.99999712</v>
+      </c>
+      <c r="R28">
+        <v>17.99999712</v>
+      </c>
+      <c r="S28">
+        <v>17.99999712</v>
+      </c>
+      <c r="T28">
+        <v>17.99999712</v>
+      </c>
+      <c r="U28">
+        <v>17.99999712</v>
+      </c>
+      <c r="V28">
+        <v>17.99999712</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>7</v>
+      </c>
+      <c r="C29" s="2">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <v>71.999988479999999</v>
+      </c>
+      <c r="G29">
+        <v>89.999985600000002</v>
+      </c>
+      <c r="H29">
+        <v>107.99998272000001</v>
+      </c>
+      <c r="I29">
+        <v>125.99997983999999</v>
+      </c>
+      <c r="J29">
+        <v>143.99997696</v>
+      </c>
+      <c r="K29">
+        <v>161.99997407999999</v>
+      </c>
+      <c r="L29" s="10">
+        <v>179.9999712</v>
+      </c>
+      <c r="M29">
+        <v>197.99996831999999</v>
+      </c>
+      <c r="N29">
+        <v>215.99996544000001</v>
+      </c>
+      <c r="O29">
+        <v>233.99996256</v>
+      </c>
+      <c r="P29">
+        <v>251.99995967999999</v>
+      </c>
+      <c r="Q29">
+        <v>269.99995680000001</v>
+      </c>
+      <c r="R29">
+        <v>287.99995392</v>
+      </c>
+      <c r="S29">
+        <v>305.99995103999998</v>
+      </c>
+      <c r="T29">
+        <v>323.99994815999997</v>
+      </c>
+      <c r="U29">
+        <v>341.99994528000002</v>
+      </c>
+      <c r="V29">
+        <v>359.99994240000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>21</v>
+      </c>
+      <c r="B30" t="s">
+        <v>5</v>
+      </c>
+      <c r="C30" s="2">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+      <c r="G30">
+        <v>0</v>
+      </c>
+      <c r="H30">
+        <v>0</v>
+      </c>
+      <c r="I30">
+        <v>0</v>
+      </c>
+      <c r="J30">
+        <v>0</v>
+      </c>
+      <c r="K30">
+        <v>0</v>
+      </c>
+      <c r="L30" s="10">
+        <v>0</v>
+      </c>
+      <c r="M30">
+        <v>0</v>
+      </c>
+      <c r="N30">
+        <v>0</v>
+      </c>
+      <c r="O30">
+        <v>0</v>
+      </c>
+      <c r="P30">
+        <v>0</v>
+      </c>
+      <c r="Q30">
+        <v>0</v>
+      </c>
+      <c r="R30">
+        <v>0</v>
+      </c>
+      <c r="S30">
+        <v>0</v>
+      </c>
+      <c r="T30">
+        <v>0</v>
+      </c>
+      <c r="U30">
+        <v>0</v>
+      </c>
+      <c r="V30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>6</v>
+      </c>
+      <c r="C31" s="2">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <v>0</v>
+      </c>
+      <c r="H31">
+        <v>0</v>
+      </c>
+      <c r="I31">
+        <v>0</v>
+      </c>
+      <c r="J31">
+        <v>0</v>
+      </c>
+      <c r="K31">
+        <v>0</v>
+      </c>
+      <c r="L31" s="10">
+        <v>0</v>
+      </c>
+      <c r="M31">
+        <v>0</v>
+      </c>
+      <c r="N31">
+        <v>0</v>
+      </c>
+      <c r="O31">
+        <v>0</v>
+      </c>
+      <c r="P31">
+        <v>0</v>
+      </c>
+      <c r="Q31">
+        <v>0</v>
+      </c>
+      <c r="R31">
+        <v>0</v>
+      </c>
+      <c r="S31">
+        <v>0</v>
+      </c>
+      <c r="T31">
+        <v>0</v>
+      </c>
+      <c r="U31">
+        <v>0</v>
+      </c>
+      <c r="V31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>7</v>
+      </c>
+      <c r="C32" s="2">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
+      <c r="G32">
+        <v>0</v>
+      </c>
+      <c r="H32">
+        <v>0</v>
+      </c>
+      <c r="I32">
+        <v>0</v>
+      </c>
+      <c r="J32">
+        <v>0</v>
+      </c>
+      <c r="K32">
+        <v>0</v>
+      </c>
+      <c r="L32" s="10">
+        <v>0</v>
+      </c>
+      <c r="M32">
+        <v>0</v>
+      </c>
+      <c r="N32">
+        <v>0</v>
+      </c>
+      <c r="O32">
+        <v>0</v>
+      </c>
+      <c r="P32">
+        <v>0</v>
+      </c>
+      <c r="Q32">
+        <v>0</v>
+      </c>
+      <c r="R32">
+        <v>0</v>
+      </c>
+      <c r="S32">
+        <v>0</v>
+      </c>
+      <c r="T32">
+        <v>0</v>
+      </c>
+      <c r="U32">
+        <v>0</v>
+      </c>
+      <c r="V32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>22</v>
+      </c>
+      <c r="B33" t="s">
+        <v>5</v>
+      </c>
+      <c r="C33" s="2">
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
+      <c r="H33">
+        <v>0</v>
+      </c>
+      <c r="I33">
+        <v>0</v>
+      </c>
+      <c r="J33">
+        <v>0</v>
+      </c>
+      <c r="K33">
+        <v>0</v>
+      </c>
+      <c r="L33" s="10">
+        <v>0</v>
+      </c>
+      <c r="M33">
+        <v>0</v>
+      </c>
+      <c r="N33">
+        <v>0</v>
+      </c>
+      <c r="O33">
+        <v>0</v>
+      </c>
+      <c r="P33">
+        <v>0</v>
+      </c>
+      <c r="Q33">
+        <v>0</v>
+      </c>
+      <c r="R33">
+        <v>0</v>
+      </c>
+      <c r="S33">
+        <v>0</v>
+      </c>
+      <c r="T33">
+        <v>0</v>
+      </c>
+      <c r="U33">
+        <v>0</v>
+      </c>
+      <c r="V33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>6</v>
+      </c>
+      <c r="C34" s="2">
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="F34">
+        <v>0</v>
+      </c>
+      <c r="G34">
+        <v>0</v>
+      </c>
+      <c r="H34">
+        <v>0</v>
+      </c>
+      <c r="I34">
+        <v>0</v>
+      </c>
+      <c r="J34">
+        <v>0</v>
+      </c>
+      <c r="K34">
+        <v>0</v>
+      </c>
+      <c r="L34" s="10">
+        <v>0</v>
+      </c>
+      <c r="M34">
+        <v>0</v>
+      </c>
+      <c r="N34">
+        <v>0</v>
+      </c>
+      <c r="O34">
+        <v>0</v>
+      </c>
+      <c r="P34">
+        <v>0</v>
+      </c>
+      <c r="Q34">
+        <v>0</v>
+      </c>
+      <c r="R34">
+        <v>0</v>
+      </c>
+      <c r="S34">
+        <v>0</v>
+      </c>
+      <c r="T34">
+        <v>0</v>
+      </c>
+      <c r="U34">
+        <v>0</v>
+      </c>
+      <c r="V34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>7</v>
+      </c>
+      <c r="C35" s="2">
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
+      </c>
+      <c r="G35">
+        <v>0</v>
+      </c>
+      <c r="H35">
+        <v>0</v>
+      </c>
+      <c r="I35">
+        <v>0</v>
+      </c>
+      <c r="J35">
+        <v>0</v>
+      </c>
+      <c r="K35">
+        <v>0</v>
+      </c>
+      <c r="L35" s="10">
+        <v>0</v>
+      </c>
+      <c r="M35">
+        <v>0</v>
+      </c>
+      <c r="N35">
+        <v>0</v>
+      </c>
+      <c r="O35">
+        <v>0</v>
+      </c>
+      <c r="P35">
+        <v>0</v>
+      </c>
+      <c r="Q35">
+        <v>0</v>
+      </c>
+      <c r="R35">
+        <v>0</v>
+      </c>
+      <c r="S35">
+        <v>0</v>
+      </c>
+      <c r="T35">
+        <v>0</v>
+      </c>
+      <c r="U35">
+        <v>0</v>
+      </c>
+      <c r="V35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>23</v>
+      </c>
+      <c r="B36" t="s">
+        <v>5</v>
+      </c>
+      <c r="C36" s="2">
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+      <c r="F36">
+        <v>0</v>
+      </c>
+      <c r="G36">
+        <v>0</v>
+      </c>
+      <c r="H36">
+        <v>0</v>
+      </c>
+      <c r="I36">
+        <v>0</v>
+      </c>
+      <c r="J36">
+        <v>0</v>
+      </c>
+      <c r="K36">
+        <v>0</v>
+      </c>
+      <c r="L36" s="10">
+        <v>0</v>
+      </c>
+      <c r="M36">
+        <v>0</v>
+      </c>
+      <c r="N36">
+        <v>0</v>
+      </c>
+      <c r="O36">
+        <v>0</v>
+      </c>
+      <c r="P36">
+        <v>0</v>
+      </c>
+      <c r="Q36">
+        <v>0</v>
+      </c>
+      <c r="R36">
+        <v>0</v>
+      </c>
+      <c r="S36">
+        <v>0</v>
+      </c>
+      <c r="T36">
+        <v>0</v>
+      </c>
+      <c r="U36">
+        <v>0</v>
+      </c>
+      <c r="V36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>6</v>
+      </c>
+      <c r="C37" s="2">
+        <v>0</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <v>0</v>
+      </c>
+      <c r="F37">
+        <v>0</v>
+      </c>
+      <c r="G37">
+        <v>0</v>
+      </c>
+      <c r="H37">
+        <v>0</v>
+      </c>
+      <c r="I37">
+        <v>0</v>
+      </c>
+      <c r="J37">
+        <v>0</v>
+      </c>
+      <c r="K37">
+        <v>0</v>
+      </c>
+      <c r="L37" s="10">
+        <v>0</v>
+      </c>
+      <c r="M37">
+        <v>0</v>
+      </c>
+      <c r="N37">
+        <v>0</v>
+      </c>
+      <c r="O37">
+        <v>0</v>
+      </c>
+      <c r="P37">
+        <v>0</v>
+      </c>
+      <c r="Q37">
+        <v>0</v>
+      </c>
+      <c r="R37">
+        <v>0</v>
+      </c>
+      <c r="S37">
+        <v>0</v>
+      </c>
+      <c r="T37">
+        <v>0</v>
+      </c>
+      <c r="U37">
+        <v>0</v>
+      </c>
+      <c r="V37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>7</v>
+      </c>
+      <c r="C38" s="2">
+        <v>0</v>
+      </c>
+      <c r="D38">
+        <v>0</v>
+      </c>
+      <c r="E38">
+        <v>0</v>
+      </c>
+      <c r="F38">
+        <v>0</v>
+      </c>
+      <c r="G38">
+        <v>0</v>
+      </c>
+      <c r="H38">
+        <v>0</v>
+      </c>
+      <c r="I38">
+        <v>0</v>
+      </c>
+      <c r="J38">
+        <v>0</v>
+      </c>
+      <c r="K38">
+        <v>0</v>
+      </c>
+      <c r="L38" s="10">
+        <v>0</v>
+      </c>
+      <c r="M38">
+        <v>0</v>
+      </c>
+      <c r="N38">
+        <v>0</v>
+      </c>
+      <c r="O38">
+        <v>0</v>
+      </c>
+      <c r="P38">
+        <v>0</v>
+      </c>
+      <c r="Q38">
+        <v>0</v>
+      </c>
+      <c r="R38">
+        <v>0</v>
+      </c>
+      <c r="S38">
+        <v>0</v>
+      </c>
+      <c r="T38">
+        <v>0</v>
+      </c>
+      <c r="U38">
+        <v>0</v>
+      </c>
+      <c r="V38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>24</v>
+      </c>
+      <c r="B39" t="s">
+        <v>5</v>
+      </c>
+      <c r="C39" s="2">
+        <v>0</v>
+      </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
+      <c r="F39">
+        <v>0</v>
+      </c>
+      <c r="G39">
+        <v>0</v>
+      </c>
+      <c r="H39">
+        <v>0</v>
+      </c>
+      <c r="I39">
+        <v>0</v>
+      </c>
+      <c r="J39">
+        <v>0</v>
+      </c>
+      <c r="K39">
+        <v>0</v>
+      </c>
+      <c r="L39" s="10">
+        <v>0</v>
+      </c>
+      <c r="M39">
+        <v>0</v>
+      </c>
+      <c r="N39">
+        <v>0</v>
+      </c>
+      <c r="O39">
+        <v>0</v>
+      </c>
+      <c r="P39">
+        <v>0</v>
+      </c>
+      <c r="Q39">
+        <v>0</v>
+      </c>
+      <c r="R39">
+        <v>0</v>
+      </c>
+      <c r="S39">
+        <v>0</v>
+      </c>
+      <c r="T39">
+        <v>0</v>
+      </c>
+      <c r="U39">
+        <v>0</v>
+      </c>
+      <c r="V39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>6</v>
+      </c>
+      <c r="C40" s="2">
+        <v>0</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+      <c r="E40">
+        <v>0</v>
+      </c>
+      <c r="F40">
+        <v>0</v>
+      </c>
+      <c r="G40">
+        <v>0</v>
+      </c>
+      <c r="H40">
+        <v>0</v>
+      </c>
+      <c r="I40">
+        <v>0</v>
+      </c>
+      <c r="J40">
+        <v>0</v>
+      </c>
+      <c r="K40">
+        <v>0</v>
+      </c>
+      <c r="L40" s="10">
+        <v>0</v>
+      </c>
+      <c r="M40">
+        <v>0</v>
+      </c>
+      <c r="N40">
+        <v>0</v>
+      </c>
+      <c r="O40">
+        <v>0</v>
+      </c>
+      <c r="P40">
+        <v>0</v>
+      </c>
+      <c r="Q40">
+        <v>0</v>
+      </c>
+      <c r="R40">
+        <v>0</v>
+      </c>
+      <c r="S40">
+        <v>0</v>
+      </c>
+      <c r="T40">
+        <v>0</v>
+      </c>
+      <c r="U40">
+        <v>0</v>
+      </c>
+      <c r="V40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>7</v>
+      </c>
+      <c r="C41" s="2">
+        <v>0</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
+      <c r="F41">
+        <v>0</v>
+      </c>
+      <c r="G41">
+        <v>0</v>
+      </c>
+      <c r="H41">
+        <v>0</v>
+      </c>
+      <c r="I41">
+        <v>0</v>
+      </c>
+      <c r="J41">
+        <v>0</v>
+      </c>
+      <c r="K41">
+        <v>0</v>
+      </c>
+      <c r="L41" s="10">
+        <v>0</v>
+      </c>
+      <c r="M41">
+        <v>0</v>
+      </c>
+      <c r="N41">
+        <v>0</v>
+      </c>
+      <c r="O41">
+        <v>0</v>
+      </c>
+      <c r="P41">
+        <v>0</v>
+      </c>
+      <c r="Q41">
+        <v>0</v>
+      </c>
+      <c r="R41">
+        <v>0</v>
+      </c>
+      <c r="S41">
+        <v>0</v>
+      </c>
+      <c r="T41">
+        <v>0</v>
+      </c>
+      <c r="U41">
+        <v>0</v>
+      </c>
+      <c r="V41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>25</v>
+      </c>
+      <c r="B42" t="s">
+        <v>5</v>
+      </c>
+      <c r="C42" s="2">
+        <v>0</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+      <c r="E42">
+        <v>0</v>
+      </c>
+      <c r="F42">
+        <v>0</v>
+      </c>
+      <c r="G42">
+        <v>0</v>
+      </c>
+      <c r="H42">
+        <v>0</v>
+      </c>
+      <c r="I42">
+        <v>0</v>
+      </c>
+      <c r="J42">
+        <v>0</v>
+      </c>
+      <c r="K42">
+        <v>0</v>
+      </c>
+      <c r="L42" s="10">
+        <v>0</v>
+      </c>
+      <c r="M42">
+        <v>0</v>
+      </c>
+      <c r="N42">
+        <v>0</v>
+      </c>
+      <c r="O42">
+        <v>0</v>
+      </c>
+      <c r="P42">
+        <v>0</v>
+      </c>
+      <c r="Q42">
+        <v>0</v>
+      </c>
+      <c r="R42">
+        <v>0</v>
+      </c>
+      <c r="S42">
+        <v>0</v>
+      </c>
+      <c r="T42">
+        <v>0</v>
+      </c>
+      <c r="U42">
+        <v>0</v>
+      </c>
+      <c r="V42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>6</v>
+      </c>
+      <c r="C43" s="2">
+        <v>0</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="E43">
+        <v>0</v>
+      </c>
+      <c r="F43">
+        <v>0</v>
+      </c>
+      <c r="G43">
+        <v>0</v>
+      </c>
+      <c r="H43">
+        <v>0</v>
+      </c>
+      <c r="I43">
+        <v>0</v>
+      </c>
+      <c r="J43">
+        <v>0</v>
+      </c>
+      <c r="K43">
+        <v>0</v>
+      </c>
+      <c r="L43" s="10">
+        <v>0</v>
+      </c>
+      <c r="M43">
+        <v>0</v>
+      </c>
+      <c r="N43">
+        <v>0</v>
+      </c>
+      <c r="O43">
+        <v>0</v>
+      </c>
+      <c r="P43">
+        <v>0</v>
+      </c>
+      <c r="Q43">
+        <v>0</v>
+      </c>
+      <c r="R43">
+        <v>0</v>
+      </c>
+      <c r="S43">
+        <v>0</v>
+      </c>
+      <c r="T43">
+        <v>0</v>
+      </c>
+      <c r="U43">
+        <v>0</v>
+      </c>
+      <c r="V43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>7</v>
+      </c>
+      <c r="C44" s="2">
+        <v>0</v>
+      </c>
+      <c r="D44">
+        <v>0</v>
+      </c>
+      <c r="E44">
+        <v>0</v>
+      </c>
+      <c r="F44">
+        <v>0</v>
+      </c>
+      <c r="G44">
+        <v>0</v>
+      </c>
+      <c r="H44">
+        <v>0</v>
+      </c>
+      <c r="I44">
+        <v>0</v>
+      </c>
+      <c r="J44">
+        <v>0</v>
+      </c>
+      <c r="K44">
+        <v>0</v>
+      </c>
+      <c r="L44" s="10">
+        <v>0</v>
+      </c>
+      <c r="M44">
+        <v>0</v>
+      </c>
+      <c r="N44">
+        <v>0</v>
+      </c>
+      <c r="O44">
+        <v>0</v>
+      </c>
+      <c r="P44">
+        <v>0</v>
+      </c>
+      <c r="Q44">
+        <v>0</v>
+      </c>
+      <c r="R44">
+        <v>0</v>
+      </c>
+      <c r="S44">
+        <v>0</v>
+      </c>
+      <c r="T44">
+        <v>0</v>
+      </c>
+      <c r="U44">
+        <v>0</v>
+      </c>
+      <c r="V44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>26</v>
+      </c>
+      <c r="B45" t="s">
+        <v>5</v>
+      </c>
+      <c r="C45" s="2">
+        <v>0</v>
+      </c>
+      <c r="D45">
+        <v>0</v>
+      </c>
+      <c r="E45">
+        <v>0</v>
+      </c>
+      <c r="F45">
+        <v>0</v>
+      </c>
+      <c r="G45">
+        <v>0</v>
+      </c>
+      <c r="H45">
+        <v>0</v>
+      </c>
+      <c r="I45">
+        <v>0</v>
+      </c>
+      <c r="J45">
+        <v>0</v>
+      </c>
+      <c r="K45">
+        <v>0</v>
+      </c>
+      <c r="L45" s="10">
+        <v>0</v>
+      </c>
+      <c r="M45">
+        <v>0</v>
+      </c>
+      <c r="N45">
+        <v>0</v>
+      </c>
+      <c r="O45">
+        <v>0</v>
+      </c>
+      <c r="P45">
+        <v>0</v>
+      </c>
+      <c r="Q45">
+        <v>0</v>
+      </c>
+      <c r="R45">
+        <v>0</v>
+      </c>
+      <c r="S45">
+        <v>0</v>
+      </c>
+      <c r="T45">
+        <v>0</v>
+      </c>
+      <c r="U45">
+        <v>0</v>
+      </c>
+      <c r="V45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>6</v>
+      </c>
+      <c r="C46" s="2">
+        <v>0</v>
+      </c>
+      <c r="D46">
+        <v>0</v>
+      </c>
+      <c r="E46">
+        <v>0</v>
+      </c>
+      <c r="F46">
+        <v>0</v>
+      </c>
+      <c r="G46">
+        <v>0</v>
+      </c>
+      <c r="H46">
+        <v>0</v>
+      </c>
+      <c r="I46">
+        <v>0</v>
+      </c>
+      <c r="J46">
+        <v>0</v>
+      </c>
+      <c r="K46">
+        <v>0</v>
+      </c>
+      <c r="L46" s="10">
+        <v>0</v>
+      </c>
+      <c r="M46">
+        <v>0</v>
+      </c>
+      <c r="N46">
+        <v>0</v>
+      </c>
+      <c r="O46">
+        <v>0</v>
+      </c>
+      <c r="P46">
+        <v>0</v>
+      </c>
+      <c r="Q46">
+        <v>0</v>
+      </c>
+      <c r="R46">
+        <v>0</v>
+      </c>
+      <c r="S46">
+        <v>0</v>
+      </c>
+      <c r="T46">
+        <v>0</v>
+      </c>
+      <c r="U46">
+        <v>0</v>
+      </c>
+      <c r="V46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>7</v>
+      </c>
+      <c r="C47" s="2">
+        <v>0</v>
+      </c>
+      <c r="D47">
+        <v>0</v>
+      </c>
+      <c r="E47">
+        <v>0</v>
+      </c>
+      <c r="F47">
+        <v>0</v>
+      </c>
+      <c r="G47">
+        <v>0</v>
+      </c>
+      <c r="H47">
+        <v>0</v>
+      </c>
+      <c r="I47">
+        <v>0</v>
+      </c>
+      <c r="J47">
+        <v>0</v>
+      </c>
+      <c r="K47">
+        <v>0</v>
+      </c>
+      <c r="L47" s="10">
+        <v>0</v>
+      </c>
+      <c r="M47">
+        <v>0</v>
+      </c>
+      <c r="N47">
+        <v>0</v>
+      </c>
+      <c r="O47">
+        <v>0</v>
+      </c>
+      <c r="P47">
+        <v>0</v>
+      </c>
+      <c r="Q47">
+        <v>0</v>
+      </c>
+      <c r="R47">
+        <v>0</v>
+      </c>
+      <c r="S47">
+        <v>0</v>
+      </c>
+      <c r="T47">
+        <v>0</v>
+      </c>
+      <c r="U47">
+        <v>0</v>
+      </c>
+      <c r="V47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>9</v>
+      </c>
+      <c r="C48" s="2">
+        <v>17.99999712</v>
+      </c>
+      <c r="D48">
+        <v>17.99999712</v>
+      </c>
+      <c r="E48">
+        <v>17.99999712</v>
+      </c>
+      <c r="F48">
+        <v>17.99999712</v>
+      </c>
+      <c r="G48">
+        <v>17.99999712</v>
+      </c>
+      <c r="H48">
+        <v>17.99999712</v>
+      </c>
+      <c r="I48">
+        <v>17.99999712</v>
+      </c>
+      <c r="J48">
+        <v>17.99999712</v>
+      </c>
+      <c r="K48">
+        <v>17.99999712</v>
+      </c>
+      <c r="L48" s="10">
+        <v>17.99999712</v>
+      </c>
+      <c r="M48">
+        <v>17.99999712</v>
+      </c>
+      <c r="N48">
+        <v>17.99999712</v>
+      </c>
+      <c r="O48">
+        <v>17.99999712</v>
+      </c>
+      <c r="P48">
+        <v>17.99999712</v>
+      </c>
+      <c r="Q48">
+        <v>17.99999712</v>
+      </c>
+      <c r="R48">
+        <v>17.99999712</v>
+      </c>
+      <c r="S48">
+        <v>17.99999712</v>
+      </c>
+      <c r="T48">
+        <v>17.99999712</v>
+      </c>
+      <c r="U48">
+        <v>17.99999712</v>
+      </c>
+      <c r="V48">
+        <v>17.99999712</v>
+      </c>
+    </row>
+    <row r="49" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>8</v>
+      </c>
+      <c r="C49" s="2">
+        <v>17.99999712</v>
+      </c>
+      <c r="D49">
+        <v>35.999994239999999</v>
+      </c>
+      <c r="E49">
+        <v>53.999991360000003</v>
+      </c>
+      <c r="F49">
+        <v>71.999988479999999</v>
+      </c>
+      <c r="G49">
+        <v>89.999985600000002</v>
+      </c>
+      <c r="H49">
+        <v>107.99998272000001</v>
+      </c>
+      <c r="I49">
+        <v>125.99997983999999</v>
+      </c>
+      <c r="J49">
+        <v>143.99997696</v>
+      </c>
+      <c r="K49">
+        <v>161.99997407999999</v>
+      </c>
+      <c r="L49" s="10">
+        <v>179.9999712</v>
+      </c>
+      <c r="M49">
+        <v>197.99996831999999</v>
+      </c>
+      <c r="N49">
+        <v>215.99996544000001</v>
+      </c>
+      <c r="O49">
+        <v>233.99996256</v>
+      </c>
+      <c r="P49">
+        <v>251.99995967999999</v>
+      </c>
+      <c r="Q49">
+        <v>269.99995680000001</v>
+      </c>
+      <c r="R49">
+        <v>287.99995392</v>
+      </c>
+      <c r="S49">
+        <v>305.99995103999998</v>
+      </c>
+      <c r="T49">
+        <v>323.99994815999997</v>
+      </c>
+      <c r="U49">
+        <v>341.99994528000002</v>
+      </c>
+      <c r="V49">
+        <v>359.99994240000001</v>
+      </c>
+    </row>
+    <row r="50" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>10</v>
+      </c>
+      <c r="C50" s="2">
+        <v>247.7653</v>
+      </c>
+      <c r="D50">
+        <v>495.53059999999999</v>
+      </c>
+      <c r="E50">
+        <v>743.29589999999996</v>
+      </c>
+      <c r="F50">
+        <v>997.71429999999998</v>
+      </c>
+      <c r="G50">
+        <v>1309.643</v>
+      </c>
+      <c r="H50">
+        <v>1621.5709999999999</v>
+      </c>
+      <c r="I50">
+        <v>1933.5</v>
+      </c>
+      <c r="J50">
+        <v>2245.4290000000001</v>
+      </c>
+      <c r="K50">
+        <v>2557.357</v>
+      </c>
+      <c r="L50" s="10">
+        <v>2869.2860000000001</v>
+      </c>
+      <c r="M50">
+        <v>3181.2139999999999</v>
+      </c>
+      <c r="N50">
+        <v>3493.143</v>
+      </c>
+      <c r="O50">
+        <v>3805.0709999999999</v>
+      </c>
+      <c r="P50">
+        <v>4117</v>
+      </c>
+      <c r="Q50">
+        <v>4428.9290000000001</v>
+      </c>
+      <c r="R50">
+        <v>4740.857</v>
+      </c>
+      <c r="S50">
+        <v>5052.7860000000001</v>
+      </c>
+      <c r="T50">
+        <v>5364.7139999999999</v>
+      </c>
+      <c r="U50">
+        <v>5676.643</v>
+      </c>
+      <c r="V50">
+        <v>5988.5709999999999</v>
+      </c>
+    </row>
+    <row r="51" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>11</v>
+      </c>
+      <c r="C51" s="2">
+        <v>359.99994240000001</v>
+      </c>
+      <c r="D51">
+        <v>719.99988480000002</v>
+      </c>
+      <c r="E51">
+        <v>1079.9998272</v>
+      </c>
+      <c r="F51">
+        <v>1439.9997696</v>
+      </c>
+      <c r="G51">
+        <v>1799.999712</v>
+      </c>
+      <c r="H51">
+        <v>2159.9996544000001</v>
+      </c>
+      <c r="I51">
+        <v>2519.9995967999998</v>
+      </c>
+      <c r="J51">
+        <v>2879.9995392000001</v>
+      </c>
+      <c r="K51">
+        <v>3239.9994815999999</v>
+      </c>
+      <c r="L51" s="10">
+        <v>3599.9994240000001</v>
+      </c>
+      <c r="M51">
+        <v>3959.9993663999999</v>
+      </c>
+      <c r="N51">
+        <v>4319.9993088000001</v>
+      </c>
+      <c r="O51">
+        <v>4679.9992511999999</v>
+      </c>
+      <c r="P51">
+        <v>5039.9991935999997</v>
+      </c>
+      <c r="Q51">
+        <v>5399.9991360000004</v>
+      </c>
+      <c r="R51">
+        <v>5759.9990784000001</v>
+      </c>
+      <c r="S51">
+        <v>6119.9990207999999</v>
+      </c>
+      <c r="T51">
+        <v>6479.9989631999997</v>
+      </c>
+      <c r="U51">
+        <v>6839.9989056000004</v>
+      </c>
+      <c r="V51">
+        <v>7199.9988480000002</v>
+      </c>
+    </row>
+    <row r="52" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>12</v>
+      </c>
+      <c r="C52" s="2">
+        <v>112.23467624</v>
+      </c>
+      <c r="D52">
+        <v>224.46935248</v>
+      </c>
+      <c r="E52">
+        <v>336.70402872</v>
+      </c>
+      <c r="F52">
+        <v>442.28568480000001</v>
+      </c>
+      <c r="G52">
+        <v>490.35710599999999</v>
+      </c>
+      <c r="H52">
+        <v>538.42852719999996</v>
+      </c>
+      <c r="I52">
+        <v>586.49994839999999</v>
+      </c>
+      <c r="J52">
+        <v>634.57136960000003</v>
+      </c>
+      <c r="K52">
+        <v>682.64279079999994</v>
+      </c>
+      <c r="L52" s="10">
+        <v>730.71421199999997</v>
+      </c>
+      <c r="M52">
+        <v>778.78563320000001</v>
+      </c>
+      <c r="N52">
+        <v>826.85705440000004</v>
+      </c>
+      <c r="O52">
+        <v>874.92847559999996</v>
+      </c>
+      <c r="P52">
+        <v>922.99989679999999</v>
+      </c>
+      <c r="Q52">
+        <v>971.07131800000002</v>
+      </c>
+      <c r="R52">
+        <v>1019.1427392000001</v>
+      </c>
+      <c r="S52">
+        <v>1067.2141604000001</v>
+      </c>
+      <c r="T52">
+        <v>1115.2855815999999</v>
+      </c>
+      <c r="U52">
+        <v>1163.3570027999999</v>
+      </c>
+      <c r="V52">
+        <v>1211.4284239999999</v>
+      </c>
+    </row>
+    <row r="55" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A55" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B55" s="10"/>
+      <c r="C55" s="14">
+        <v>20000000</v>
+      </c>
+      <c r="D55" s="14"/>
+    </row>
+    <row r="56" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A56" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C56" s="15">
+        <v>5</v>
+      </c>
+      <c r="D56" s="15"/>
+    </row>
+    <row r="57" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A57" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C57" s="15">
+        <v>18</v>
+      </c>
+      <c r="D57" s="15"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="C55:D55"/>
+    <mergeCell ref="C56:D56"/>
+    <mergeCell ref="C57:D57"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
@@ -7058,8 +10538,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:AF27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B39" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>